<commit_message>
Adding Cup Sensor state logic.
</commit_message>
<xml_diff>
--- a/Docs/LCD_Telas.xlsx
+++ b/Docs/LCD_Telas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\victo\Documents\ShakeBuilder\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9FF43C8-A0E1-445A-B031-D85A1119E1FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84DAD127-2FF6-4F82-AC68-21351A750FBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{F931B482-B22E-4A8C-BDA0-770A01F35DF1}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="58">
   <si>
     <t>P</t>
   </si>
@@ -207,6 +207,9 @@
   </si>
   <si>
     <t>Servindo shake</t>
+  </si>
+  <si>
+    <t>FIM</t>
   </si>
 </sst>
 </file>
@@ -230,7 +233,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -264,11 +267,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -277,13 +289,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -600,10 +615,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F8F3978-6515-466E-81D1-DEBCCCC0888F}">
-  <dimension ref="A1:AQ22"/>
+  <dimension ref="A1:AQ29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V19" sqref="V19"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="Z30" sqref="Z30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -612,30 +627,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
-      <c r="AC1" s="4" t="s">
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
+      <c r="AC1" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="AD1" s="4"/>
-      <c r="AE1" s="4"/>
-      <c r="AF1" s="4"/>
-      <c r="AG1" s="4"/>
-      <c r="AH1" s="4"/>
-      <c r="AI1" s="4"/>
-      <c r="AJ1" s="4"/>
-      <c r="AK1" s="4"/>
-      <c r="AL1" s="4"/>
+      <c r="AD1" s="6"/>
+      <c r="AE1" s="6"/>
+      <c r="AF1" s="6"/>
+      <c r="AG1" s="6"/>
+      <c r="AH1" s="6"/>
+      <c r="AI1" s="6"/>
+      <c r="AJ1" s="6"/>
+      <c r="AK1" s="6"/>
+      <c r="AL1" s="6"/>
     </row>
     <row r="2" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
@@ -782,10 +797,10 @@
       <c r="J3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="K3" s="6" t="s">
+      <c r="K3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="L3" s="6" t="s">
+      <c r="L3" s="5" t="s">
         <v>43</v>
       </c>
       <c r="M3" s="2" t="s">
@@ -1201,30 +1216,30 @@
       </c>
     </row>
     <row r="9" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="F9" s="4" t="s">
+      <c r="F9" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
-      <c r="L9" s="4"/>
-      <c r="M9" s="4"/>
-      <c r="N9" s="4"/>
-      <c r="O9" s="4"/>
-      <c r="AC9" s="4" t="s">
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="6"/>
+      <c r="N9" s="6"/>
+      <c r="O9" s="6"/>
+      <c r="AC9" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="AD9" s="4"/>
-      <c r="AE9" s="4"/>
-      <c r="AF9" s="4"/>
-      <c r="AG9" s="4"/>
-      <c r="AH9" s="4"/>
-      <c r="AI9" s="4"/>
-      <c r="AJ9" s="4"/>
-      <c r="AK9" s="4"/>
-      <c r="AL9" s="4"/>
+      <c r="AD9" s="6"/>
+      <c r="AE9" s="6"/>
+      <c r="AF9" s="6"/>
+      <c r="AG9" s="6"/>
+      <c r="AH9" s="6"/>
+      <c r="AI9" s="6"/>
+      <c r="AJ9" s="6"/>
+      <c r="AK9" s="6"/>
+      <c r="AL9" s="6"/>
     </row>
     <row r="10" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
@@ -1409,6 +1424,9 @@
       <c r="T11" s="2" t="s">
         <v>31</v>
       </c>
+      <c r="V11">
+        <v>0</v>
+      </c>
       <c r="X11" s="2" t="s">
         <v>31</v>
       </c>
@@ -1531,6 +1549,9 @@
       <c r="T12" s="2" t="s">
         <v>23</v>
       </c>
+      <c r="V12">
+        <v>1</v>
+      </c>
       <c r="X12" s="2" t="s">
         <v>16</v>
       </c>
@@ -1546,7 +1567,7 @@
       <c r="AB12" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="AC12" s="5" t="s">
+      <c r="AC12" s="4" t="s">
         <v>40</v>
       </c>
       <c r="AD12" s="2" t="s">
@@ -1613,6 +1634,9 @@
       <c r="R13" s="2"/>
       <c r="S13" s="2"/>
       <c r="T13" s="2"/>
+      <c r="V13">
+        <v>2</v>
+      </c>
       <c r="X13" s="2" t="s">
         <v>32</v>
       </c>
@@ -1735,6 +1759,9 @@
       <c r="T14" s="2" t="s">
         <v>31</v>
       </c>
+      <c r="V14">
+        <v>3</v>
+      </c>
       <c r="X14" s="2" t="s">
         <v>31</v>
       </c>
@@ -1797,30 +1824,30 @@
       </c>
     </row>
     <row r="17" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="F17" s="4" t="s">
+      <c r="F17" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
-      <c r="J17" s="4"/>
-      <c r="K17" s="4"/>
-      <c r="L17" s="4"/>
-      <c r="M17" s="4"/>
-      <c r="N17" s="4"/>
-      <c r="O17" s="4"/>
-      <c r="AC17" s="4" t="s">
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="6"/>
+      <c r="K17" s="6"/>
+      <c r="L17" s="6"/>
+      <c r="M17" s="6"/>
+      <c r="N17" s="6"/>
+      <c r="O17" s="6"/>
+      <c r="AC17" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="AD17" s="4"/>
-      <c r="AE17" s="4"/>
-      <c r="AF17" s="4"/>
-      <c r="AG17" s="4"/>
-      <c r="AH17" s="4"/>
-      <c r="AI17" s="4"/>
-      <c r="AJ17" s="4"/>
-      <c r="AK17" s="4"/>
-      <c r="AL17" s="4"/>
+      <c r="AD17" s="6"/>
+      <c r="AE17" s="6"/>
+      <c r="AF17" s="6"/>
+      <c r="AG17" s="6"/>
+      <c r="AH17" s="6"/>
+      <c r="AI17" s="6"/>
+      <c r="AJ17" s="6"/>
+      <c r="AK17" s="6"/>
+      <c r="AL17" s="6"/>
     </row>
     <row r="18" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
@@ -2004,6 +2031,9 @@
       </c>
       <c r="T19" s="2" t="s">
         <v>31</v>
+      </c>
+      <c r="V19">
+        <v>0</v>
       </c>
       <c r="X19" s="2" t="s">
         <v>31</v>
@@ -2104,6 +2134,9 @@
       <c r="R20" s="1"/>
       <c r="S20" s="1"/>
       <c r="T20" s="1"/>
+      <c r="V20">
+        <v>1</v>
+      </c>
       <c r="X20" s="2"/>
       <c r="Y20" s="2"/>
       <c r="Z20" s="2"/>
@@ -2184,6 +2217,9 @@
       <c r="R21" s="2"/>
       <c r="S21" s="2"/>
       <c r="T21" s="2"/>
+      <c r="V21">
+        <v>2</v>
+      </c>
       <c r="X21" s="2"/>
       <c r="Y21" s="2"/>
       <c r="Z21" s="2"/>
@@ -2281,6 +2317,9 @@
       <c r="T22" s="2" t="s">
         <v>31</v>
       </c>
+      <c r="V22">
+        <v>3</v>
+      </c>
       <c r="X22" s="2" t="s">
         <v>31</v>
       </c>
@@ -2342,8 +2381,311 @@
         <v>31</v>
       </c>
     </row>
+    <row r="24" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="F24" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
+      <c r="J24" s="6"/>
+      <c r="K24" s="6"/>
+      <c r="L24" s="6"/>
+      <c r="M24" s="6"/>
+      <c r="N24" s="6"/>
+      <c r="O24" s="6"/>
+    </row>
+    <row r="25" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A25" s="3">
+        <v>0</v>
+      </c>
+      <c r="B25" s="3">
+        <v>1</v>
+      </c>
+      <c r="C25" s="3">
+        <v>2</v>
+      </c>
+      <c r="D25" s="3">
+        <v>3</v>
+      </c>
+      <c r="E25" s="3">
+        <v>4</v>
+      </c>
+      <c r="F25" s="3">
+        <v>5</v>
+      </c>
+      <c r="G25" s="3">
+        <v>6</v>
+      </c>
+      <c r="H25" s="3">
+        <v>7</v>
+      </c>
+      <c r="I25" s="3">
+        <v>8</v>
+      </c>
+      <c r="J25" s="3">
+        <v>9</v>
+      </c>
+      <c r="K25" s="3">
+        <v>10</v>
+      </c>
+      <c r="L25" s="3">
+        <v>11</v>
+      </c>
+      <c r="M25" s="3">
+        <v>12</v>
+      </c>
+      <c r="N25" s="3">
+        <v>13</v>
+      </c>
+      <c r="O25" s="3">
+        <v>14</v>
+      </c>
+      <c r="P25" s="3">
+        <v>15</v>
+      </c>
+      <c r="Q25" s="3">
+        <v>16</v>
+      </c>
+      <c r="R25" s="3">
+        <v>17</v>
+      </c>
+      <c r="S25" s="3">
+        <v>18</v>
+      </c>
+      <c r="T25" s="3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I26" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J26" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K26" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="L26" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="M26" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="N26" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="O26" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="P26" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q26" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="R26" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="S26" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="T26" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="V26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A27" s="2"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D27" t="s">
+        <v>45</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I27" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="J27" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="K27" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L27" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="M27" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="O27" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="P27" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q27" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="R27" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="S27" s="1"/>
+      <c r="T27" s="1"/>
+      <c r="V27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A28" s="2"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I28" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J28" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="K28" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="L28" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="M28" s="2"/>
+      <c r="N28" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="O28" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q28" s="2"/>
+      <c r="R28" s="2"/>
+      <c r="S28" s="2"/>
+      <c r="T28" s="2"/>
+      <c r="V28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I29" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J29" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K29" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="L29" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="M29" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="N29" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="O29" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="P29" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q29" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="R29" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="S29" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="T29" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="V29">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
+    <mergeCell ref="F24:O24"/>
     <mergeCell ref="F1:O1"/>
     <mergeCell ref="AC1:AL1"/>
     <mergeCell ref="F9:O9"/>

</xml_diff>